<commit_message>
the previous commit message was wrong, the new commit message is : remove a spelling mistake in a row
</commit_message>
<xml_diff>
--- a/Requirements/Lhub_SIQ.xlsx
+++ b/Requirements/Lhub_SIQ.xlsx
@@ -882,14 +882,14 @@
   <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="1"/>
     <col min="2" max="2" width="69.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="92.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="102.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="13" bestFit="1" customWidth="1"/>

</xml_diff>